<commit_message>
updated test cases and summary report
</commit_message>
<xml_diff>
--- a/docs/testCases/firstSprint/12.TestCase-Contacts-Partners.xlsx
+++ b/docs/testCases/firstSprint/12.TestCase-Contacts-Partners.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vartotojas\Desktop\assets\TetsCase\TestCase-Contacts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projektas\StrangerTeam_PayApi_Project\docs\testCases\firstSprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE653C8E-6C36-404D-BA3E-63C44C29A4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626D8A90-6C0D-4D5E-87AF-0F352A4821BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="1140" windowWidth="29610" windowHeight="19455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9045" yWindow="5250" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,21 +323,56 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -352,51 +387,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A23" sqref="A23:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,46 +690,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="30" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="32"/>
+      <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -745,10 +745,10 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -773,29 +773,29 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35">
+      <c r="E6" s="22"/>
+      <c r="F6" s="23">
         <v>45261</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="30" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="29" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="29"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -823,127 +823,127 @@
       <c r="F8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>1</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="2"/>
       <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="2"/>
       <c r="F10" s="9">
         <v>2</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="2"/>
       <c r="F11" s="9">
         <v>3</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="2"/>
       <c r="F12" s="9">
         <v>4</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="2"/>
       <c r="F13" s="9">
         <v>5</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>6</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="2"/>
       <c r="F14" s="9">
         <v>6</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
@@ -976,157 +976,143 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="21" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="18" t="s">
+      <c r="E18" s="33"/>
+      <c r="F18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="18" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
     </row>
     <row r="20" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>1</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="36"/>
+      <c r="D20" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="35"/>
+      <c r="F20" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="14" t="s">
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>2</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="37"/>
+      <c r="D21" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="14" t="s">
+      <c r="E21" s="35"/>
+      <c r="F21" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="14" t="s">
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>3</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="37"/>
+      <c r="D22" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="14" t="s">
+      <c r="E22" s="35"/>
+      <c r="F22" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="14" t="s">
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>4</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>5</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="16"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>6</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="45">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="I18:K19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1141,49 +1127,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="I18:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:K25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>